<commit_message>
changes for statements in db  (#80)
* Update README.md

* first commit

* electron fixes

* bug fixes in package.json

* fixed update of main.js

* UI changes

* UI Changes 2.0

* change of sidebar

* Sidebar Changes

* changes in breadcrumbs and ui of ind. dash

* breadcrumb change

* eligibility ui change

* Summary Data Changes

* changes in db

* changes in gen report

* gem report merge changes

* changes in gen report -- 21-01-2025

* git push delete fille

* delete file

* EOD Balance added and displayed

* backend -- Summary + EOD

* failed statements db

* info button fetch data

* changes merge

* changes in gen report --2912025

* chanegs in code in gen report

* name acc manager table width  change

* gen report + rr

* generate report code changes regarding tmp folder

---------

Co-authored-by: Aiyaz17 <68592281+Aiyaz17@users.noreply.github.com>
Co-authored-by: Rajaa786 <101792809+Rajaa786@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/backend/Final_Category.xlsx
+++ b/backend/Final_Category.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$D$2362</definedName>

</xml_diff>